<commit_message>
subject and chapter api added
</commit_message>
<xml_diff>
--- a/edus project timeline and cost 17-april-2025.xlsx
+++ b/edus project timeline and cost 17-april-2025.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="123">
   <si>
     <t>admin_permissions</t>
   </si>
@@ -207,15 +207,6 @@
     <t>Add/edit/remove/block  - user</t>
   </si>
   <si>
-    <t>Add/remove - chapter in user account</t>
-  </si>
-  <si>
-    <t>Add/remove - subject in user account</t>
-  </si>
-  <si>
-    <t>Add/remove - full class in user account</t>
-  </si>
-  <si>
     <t>User</t>
   </si>
   <si>
@@ -397,6 +388,18 @@
   </si>
   <si>
     <t>Add Create super_amdin and admin and users</t>
+  </si>
+  <si>
+    <t>Total APIs</t>
+  </si>
+  <si>
+    <t>Add/remove - Full class in user account</t>
+  </si>
+  <si>
+    <t>Add/remove - Subject in user account</t>
+  </si>
+  <si>
+    <t>Add/remove - Chapter in user account</t>
   </si>
 </sst>
 </file>
@@ -465,7 +468,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -525,8 +528,26 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -615,21 +636,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -642,9 +654,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -680,10 +689,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -714,21 +727,17 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -768,7 +777,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" tooltip="Add to Favorites"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1124,184 +1133,184 @@
   <sheetData>
     <row r="1" spans="2:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="24"/>
+    </row>
+    <row r="3" spans="2:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="23"/>
-    </row>
-    <row r="3" spans="2:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="17" t="s">
+    </row>
+    <row r="24" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="16" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="17" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="17" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1348,7 +1357,7 @@
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="28" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1357,22 +1366,22 @@
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="28"/>
+      <c r="B6" s="29"/>
       <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="28"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="28"/>
-      <c r="C8" s="24" t="s">
+      <c r="B8" s="29"/>
+      <c r="C8" s="25" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -1380,69 +1389,69 @@
       </c>
     </row>
     <row r="9" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="28"/>
-      <c r="C9" s="25"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="26"/>
       <c r="D9" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="28"/>
-      <c r="C10" s="25"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="28"/>
-      <c r="C11" s="25"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="26"/>
       <c r="D11" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="28"/>
-      <c r="C12" s="25"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="26"/>
       <c r="D12" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="28"/>
-      <c r="C13" s="25"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="26"/>
       <c r="D13" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="28"/>
-      <c r="C14" s="25"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="28"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="7"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="6"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="28"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="7" t="s">
+      <c r="B16" s="29"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="19" t="s">
-        <v>117</v>
+      <c r="C17" s="18" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21" s="8">
+      <c r="B21" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="7">
         <v>15</v>
       </c>
     </row>
@@ -1472,7 +1481,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="30" t="s">
         <v>45</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -1480,46 +1489,46 @@
       </c>
     </row>
     <row r="3" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="29"/>
+      <c r="C3" s="30"/>
       <c r="D3" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="29"/>
+      <c r="C4" s="30"/>
       <c r="D4" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="29"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="29"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="29"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C8" s="4"/>
-      <c r="D8" s="18" t="s">
-        <v>117</v>
+      <c r="D8" s="17" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C9" s="4"/>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="30" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -1527,25 +1536,25 @@
       </c>
     </row>
     <row r="11" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="29"/>
+      <c r="C11" s="30"/>
       <c r="D11" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="29"/>
+      <c r="C12" s="30"/>
       <c r="D12" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="29"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="16" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="31" t="s">
         <v>33</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -1553,58 +1562,58 @@
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="31"/>
+      <c r="C17" s="32"/>
       <c r="D17" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="31"/>
+      <c r="C18" s="32"/>
       <c r="D18" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" s="31"/>
+      <c r="C19" s="32"/>
       <c r="D19" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="31"/>
+      <c r="C20" s="32"/>
       <c r="D20" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" s="31"/>
+      <c r="C21" s="32"/>
       <c r="D21" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="31"/>
+      <c r="C22" s="32"/>
       <c r="D22" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C23" s="31"/>
+      <c r="C23" s="32"/>
       <c r="D23" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C24" s="31"/>
+      <c r="C24" s="32"/>
       <c r="D24" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="3:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D27" s="9">
+      <c r="C27" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="8">
         <v>20</v>
       </c>
     </row>
@@ -1620,224 +1629,375 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:F38"/>
+  <dimension ref="C3:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="35.7109375" customWidth="1"/>
     <col min="4" max="4" width="51.28515625" customWidth="1"/>
-    <col min="6" max="6" width="25" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D3" s="6" t="s">
+    <row r="3" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C3" s="20"/>
+      <c r="D3" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C4" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C4" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="F4" s="21">
+      <c r="E4" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="F4" s="36">
+        <v>2</v>
+      </c>
+      <c r="G4" s="35">
         <v>45764</v>
       </c>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C5" s="35"/>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="34"/>
       <c r="D5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="F5" s="21">
+      <c r="E5" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" s="36">
+        <v>4</v>
+      </c>
+      <c r="G5" s="35">
         <v>45764</v>
       </c>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="35"/>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="34"/>
       <c r="D6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="F6" s="21">
+      <c r="E6" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="F6" s="36">
+        <v>4</v>
+      </c>
+      <c r="G6" s="35">
         <v>45764</v>
       </c>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C7" s="35"/>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="34"/>
       <c r="D7" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="35"/>
+      <c r="E7" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" s="36">
+        <v>4</v>
+      </c>
+      <c r="G7" s="35">
+        <v>45764</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="34"/>
       <c r="D8" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="35"/>
+      <c r="E8" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="F8" s="36">
+        <v>4</v>
+      </c>
+      <c r="G8" s="37">
+        <v>45765</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="34"/>
       <c r="D9" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="35"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="35"/>
-      <c r="D11" s="1" t="s">
+      <c r="E9" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="F9" s="36">
+        <v>4</v>
+      </c>
+      <c r="G9" s="37">
+        <v>45765</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="34"/>
+      <c r="D10" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="35"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="35"/>
+      <c r="E10" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="F10" s="36">
+        <v>1</v>
+      </c>
+      <c r="G10" s="37">
+        <v>45765</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="34"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="34"/>
+      <c r="D12" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="34"/>
       <c r="D13" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="34"/>
+      <c r="D14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="33" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="35"/>
-      <c r="D14" s="1" t="s">
+      <c r="D18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="33"/>
+      <c r="D19" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="36"/>
-      <c r="D15" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="33"/>
       <c r="D20" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="33"/>
       <c r="D21" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="33"/>
       <c r="D22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C23" s="33"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C24" s="33"/>
+      <c r="D24" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C23" s="33"/>
-      <c r="D23" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C24" s="33"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="33"/>
       <c r="D25" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26" s="33"/>
       <c r="D26" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C27" s="33"/>
-      <c r="D27" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C28" s="33"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C29" s="33"/>
       <c r="D29" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C30" s="33"/>
       <c r="D30" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C31" s="33"/>
       <c r="D31" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C32" s="33"/>
       <c r="D32" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33" s="33"/>
       <c r="D33" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34" s="34"/>
-      <c r="D34" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="38" spans="3:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D38" s="9">
+        <v>71</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+    </row>
+    <row r="37" spans="3:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" s="8">
         <v>12</v>
       </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C19:C34"/>
-    <mergeCell ref="C4:C15"/>
+    <mergeCell ref="C18:C33"/>
+    <mergeCell ref="C4:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1858,60 +2018,60 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="3:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" s="12" t="s">
+    <row r="8" spans="3:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="9" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="7" spans="3:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="10" t="s">
+      <c r="D8" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D7" s="12" t="s">
+    </row>
+    <row r="9" spans="3:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="9" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="3:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="10" t="s">
+      <c r="D9" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="3:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="12" spans="3:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="11">
+      <c r="C12" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="10">
         <f>SUM(20,12,15)</f>
         <v>47</v>
       </c>
     </row>
     <row r="14" spans="3:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>112</v>
+      <c r="C14" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Buy and user login api / documentation
</commit_message>
<xml_diff>
--- a/edus project timeline and cost 17-april-2025.xlsx
+++ b/edus project timeline and cost 17-april-2025.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="126">
   <si>
     <t>admin_permissions</t>
   </si>
@@ -393,20 +393,29 @@
     <t>Total APIs</t>
   </si>
   <si>
-    <t>Add/remove - Full class in user account</t>
-  </si>
-  <si>
-    <t>Add/remove - Subject in user account</t>
-  </si>
-  <si>
-    <t>Add/remove - Chapter in user account</t>
+    <t>remove - Chapter in user account</t>
+  </si>
+  <si>
+    <t>remove - Subject in user account</t>
+  </si>
+  <si>
+    <t>remove - Full class in user account</t>
+  </si>
+  <si>
+    <t>Add/update - Chapter in user account</t>
+  </si>
+  <si>
+    <t>Add/update - Subject in user account</t>
+  </si>
+  <si>
+    <t>Add/update - Full class in user account</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -463,6 +472,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -542,7 +558,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -641,7 +657,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -689,14 +705,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -727,17 +741,33 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -777,7 +807,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" tooltip="Add to Favorites"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1632,29 +1662,30 @@
   <dimension ref="C3:G37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="35.7109375" customWidth="1"/>
     <col min="4" max="4" width="51.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
     <col min="7" max="7" width="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C3" s="20"/>
-      <c r="D3" s="21" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="20" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1665,13 +1696,13 @@
       <c r="D4" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="F4" s="36">
+      <c r="F4" s="37">
         <v>2</v>
       </c>
-      <c r="G4" s="35">
+      <c r="G4" s="38">
         <v>45764</v>
       </c>
     </row>
@@ -1680,13 +1711,13 @@
       <c r="D5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="F5" s="36">
+      <c r="F5" s="37">
         <v>4</v>
       </c>
-      <c r="G5" s="35">
+      <c r="G5" s="38">
         <v>45764</v>
       </c>
     </row>
@@ -1695,13 +1726,13 @@
       <c r="D6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="F6" s="36">
+      <c r="F6" s="37">
         <v>4</v>
       </c>
-      <c r="G6" s="35">
+      <c r="G6" s="38">
         <v>45764</v>
       </c>
     </row>
@@ -1710,13 +1741,13 @@
       <c r="D7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="F7" s="36">
+      <c r="F7" s="37">
         <v>4</v>
       </c>
-      <c r="G7" s="35">
+      <c r="G7" s="38">
         <v>45764</v>
       </c>
     </row>
@@ -1725,13 +1756,13 @@
       <c r="D8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="F8" s="36">
+      <c r="F8" s="39">
         <v>4</v>
       </c>
-      <c r="G8" s="37">
+      <c r="G8" s="22">
         <v>45765</v>
       </c>
     </row>
@@ -1740,13 +1771,13 @@
       <c r="D9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="F9" s="36">
+      <c r="F9" s="39">
         <v>4</v>
       </c>
-      <c r="G9" s="37">
+      <c r="G9" s="22">
         <v>45765</v>
       </c>
     </row>
@@ -1755,70 +1786,112 @@
       <c r="D10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="F10" s="36">
+      <c r="F10" s="39">
         <v>1</v>
       </c>
-      <c r="G10" s="37">
+      <c r="G10" s="22">
         <v>45765</v>
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C11" s="34"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" s="36">
+        <v>1</v>
+      </c>
+      <c r="G11" s="35">
+        <v>45768</v>
+      </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C12" s="34"/>
       <c r="D12" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+        <v>124</v>
+      </c>
+      <c r="E12" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" s="36">
+        <v>1</v>
+      </c>
+      <c r="G12" s="35">
+        <v>45768</v>
+      </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C13" s="34"/>
       <c r="D13" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+        <v>125</v>
+      </c>
+      <c r="E13" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="36">
+        <v>1</v>
+      </c>
+      <c r="G13" s="35">
+        <v>45768</v>
+      </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C14" s="34"/>
       <c r="D14" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="E14" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="F14" s="36">
+        <v>1</v>
+      </c>
+      <c r="G14" s="35">
+        <v>45768</v>
+      </c>
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E15" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="F15" s="36">
+        <v>1</v>
+      </c>
+      <c r="G15" s="35">
+        <v>45768</v>
+      </c>
     </row>
     <row r="16" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="F16" s="36">
+        <v>1</v>
+      </c>
+      <c r="G16" s="35">
+        <v>45768</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="33" t="s">
@@ -1827,45 +1900,75 @@
       <c r="D18" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="E18" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" s="36">
+        <v>1</v>
+      </c>
+      <c r="G18" s="35">
+        <v>45768</v>
+      </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="33"/>
       <c r="D19" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="E19" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="F19" s="36">
+        <v>1</v>
+      </c>
+      <c r="G19" s="35">
+        <v>45768</v>
+      </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="33"/>
       <c r="D20" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="E20" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" s="36">
+        <v>1</v>
+      </c>
+      <c r="G20" s="35">
+        <v>45768</v>
+      </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="33"/>
       <c r="D21" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="E21" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="F21" s="36">
+        <v>1</v>
+      </c>
+      <c r="G21" s="35">
+        <v>45768</v>
+      </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="33"/>
       <c r="D22" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="E22" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="F22" s="36">
+        <v>1</v>
+      </c>
+      <c r="G22" s="35">
+        <v>45768</v>
+      </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="33"/>
@@ -1963,27 +2066,27 @@
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-    </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
-    </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-    </row>
-    <row r="37" spans="3:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+    </row>
+    <row r="35" spans="3:7" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+    </row>
+    <row r="36" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+    </row>
+    <row r="37" spans="3:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C37" s="8" t="s">
         <v>72</v>
       </c>
@@ -1997,9 +2100,10 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C18:C33"/>
-    <mergeCell ref="C4:C14"/>
+    <mergeCell ref="C4:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>